<commit_message>
Fixed the consistence issues across files
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
   <si>
     <t>#</t>
   </si>
@@ -29,6 +29,9 @@
     <t>Last Modified By</t>
   </si>
   <si>
+    <t>Last Modified Date</t>
+  </si>
+  <si>
     <t>File Extension</t>
   </si>
   <si>
@@ -74,7 +77,13 @@
     <t>D:\Infosys\PWC\excel-to-appscript\workspace\eclipse\google\.\excel\client\Client BB - Complex data workbook.xlsm</t>
   </si>
   <si>
-    <t>-</t>
+    <t>example</t>
+  </si>
+  <si>
+    <t>Andrew Gottesman</t>
+  </si>
+  <si>
+    <t>Tue Aug 11 05:34:13 IST 2015</t>
   </si>
   <si>
     <t>xlsm</t>
@@ -89,12 +98,24 @@
     <t>D:\Infosys\PWC\excel-to-appscript\workspace\eclipse\google\.\excel\client\ClientZZ Template (DRAFT) v1.40_CONVERSION_TESTING.xlsm</t>
   </si>
   <si>
+    <t>Corey J. Gallon</t>
+  </si>
+  <si>
+    <t>Fri Aug 14 22:10:40 IST 2015</t>
+  </si>
+  <si>
     <t>Estimatesv1.0.xlsx</t>
   </si>
   <si>
     <t>D:\Infosys\PWC\excel-to-appscript\workspace\eclipse\google\.\excel\generic\Estimatesv1.0.xlsx</t>
   </si>
   <si>
+    <t>NagaKishore Byr</t>
+  </si>
+  <si>
+    <t>Wed Nov 02 17:17:23 IST 2016</t>
+  </si>
+  <si>
     <t>xlsx</t>
   </si>
   <si>
@@ -104,18 +125,33 @@
     <t>D:\Infosys\PWC\excel-to-appscript\workspace\eclipse\google\.\excel\generic\Estimation.xlsx</t>
   </si>
   <si>
+    <t>Srinivas Kandula</t>
+  </si>
+  <si>
+    <t>Mon Oct 31 10:32:21 IST 2016</t>
+  </si>
+  <si>
     <t>myEQM-end-new.xlsx</t>
   </si>
   <si>
     <t>D:\Infosys\PWC\excel-to-appscript\workspace\eclipse\google\.\excel\special\myEQM-end-new.xlsx</t>
   </si>
   <si>
+    <t>Michael McGraw-Herdeg</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 20:10:05 IST 2017</t>
+  </si>
+  <si>
     <t>myEQM-end.xls</t>
   </si>
   <si>
     <t>D:\Infosys\PWC\excel-to-appscript\workspace\eclipse\google\.\excel\special\myEQM-end.xls</t>
   </si>
   <si>
+    <t>Thu Jan 19 20:10:24 IST 2017</t>
+  </si>
+  <si>
     <t>xls</t>
   </si>
   <si>
@@ -125,34 +161,55 @@
     <t>D:\Infosys\PWC\excel-to-appscript\workspace\eclipse\google\.\excel\special\object-embedded-new.xlsx</t>
   </si>
   <si>
+    <t>Thu Jan 19 20:28:17 IST 2017</t>
+  </si>
+  <si>
     <t>object-embedded.xls</t>
   </si>
   <si>
     <t>D:\Infosys\PWC\excel-to-appscript\workspace\eclipse\google\.\excel\special\object-embedded.xls</t>
   </si>
   <si>
+    <t>Thu Jan 19 20:32:29 IST 2017</t>
+  </si>
+  <si>
     <t>picture-embedded-new.xlsx</t>
   </si>
   <si>
     <t>D:\Infosys\PWC\excel-to-appscript\workspace\eclipse\google\.\excel\special\picture-embedded-new.xlsx</t>
   </si>
   <si>
+    <t>Thu Jan 19 20:21:43 IST 2017</t>
+  </si>
+  <si>
     <t>picture-embedded.xls</t>
   </si>
   <si>
     <t>D:\Infosys\PWC\excel-to-appscript\workspace\eclipse\google\.\excel\special\picture-embedded.xls</t>
   </si>
   <si>
+    <t>Thu Jan 19 20:21:58 IST 2017</t>
+  </si>
+  <si>
     <t>pivot-tables-new.xlsx</t>
   </si>
   <si>
     <t>D:\Infosys\PWC\excel-to-appscript\workspace\eclipse\google\.\excel\special\pivot-tables-new.xlsx</t>
   </si>
   <si>
+    <t>excel-easy.com</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 20:00:25 IST 2017</t>
+  </si>
+  <si>
     <t>pivot-tables.xls</t>
   </si>
   <si>
     <t>D:\Infosys\PWC\excel-to-appscript\workspace\eclipse\google\.\excel\special\pivot-tables.xls</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 20:00:06 IST 2017</t>
   </si>
 </sst>
 </file>
@@ -275,61 +332,67 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="b">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
       </c>
       <c r="H2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
       </c>
-      <c r="J2" t="n">
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
         <v>899572.0</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>14.0</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>11937.0</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>23.0</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>5729.0</v>
       </c>
-      <c r="O2" t="n">
-        <v>0.0</v>
-      </c>
       <c r="P2" t="n">
         <v>0.0</v>
       </c>
       <c r="Q2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R2" t="n">
         <v>3.0</v>
       </c>
-      <c r="R2" t="s">
-        <v>22</v>
+      <c r="S2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3">
@@ -337,55 +400,58 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="b">
-        <v>0</v>
-      </c>
       <c r="H3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
       </c>
-      <c r="J3" t="n">
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="n">
         <v>505814.0</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>19.0</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>3323.0</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>11.0</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>2487.0</v>
       </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
         <v>3.0</v>
       </c>
-      <c r="P3" t="n">
-        <v>0.0</v>
-      </c>
       <c r="Q3" t="n">
         <v>0.0</v>
       </c>
-      <c r="R3" t="s">
-        <v>22</v>
+      <c r="R3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4">
@@ -393,41 +459,41 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" t="b">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
       </c>
       <c r="I4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
         <v>16085.0</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>3.0</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>57.0</v>
       </c>
-      <c r="M4" t="n">
-        <v>0.0</v>
-      </c>
       <c r="N4" t="n">
         <v>0.0</v>
       </c>
@@ -440,8 +506,11 @@
       <c r="Q4" t="n">
         <v>0.0</v>
       </c>
-      <c r="R4" t="s">
-        <v>22</v>
+      <c r="R4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5">
@@ -449,41 +518,41 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" t="b">
-        <v>0</v>
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
       </c>
       <c r="I5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" t="n">
         <v>12236.0</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>2.0</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>38.0</v>
       </c>
-      <c r="M5" t="n">
-        <v>0.0</v>
-      </c>
       <c r="N5" t="n">
         <v>0.0</v>
       </c>
@@ -496,8 +565,11 @@
       <c r="Q5" t="n">
         <v>0.0</v>
       </c>
-      <c r="R5" t="s">
-        <v>22</v>
+      <c r="R5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6">
@@ -505,41 +577,41 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" t="b">
-        <v>0</v>
+        <v>42</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
       </c>
       <c r="I6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="n">
         <v>18789.0</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>2.0</v>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="n">
         <v>43.0</v>
       </c>
-      <c r="M6" t="n">
-        <v>0.0</v>
-      </c>
       <c r="N6" t="n">
         <v>0.0</v>
       </c>
@@ -552,8 +624,11 @@
       <c r="Q6" t="n">
         <v>0.0</v>
       </c>
-      <c r="R6" t="s">
-        <v>22</v>
+      <c r="R6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7">
@@ -561,41 +636,41 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" t="b">
-        <v>1</v>
+        <v>45</v>
+      </c>
+      <c r="G7" t="s">
+        <v>46</v>
       </c>
       <c r="H7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" t="n">
         <v>39936.0</v>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>2.0</v>
       </c>
-      <c r="L7" t="n">
+      <c r="M7" t="n">
         <v>43.0</v>
       </c>
-      <c r="M7" t="n">
-        <v>0.0</v>
-      </c>
       <c r="N7" t="n">
         <v>0.0</v>
       </c>
@@ -608,8 +683,11 @@
       <c r="Q7" t="n">
         <v>0.0</v>
       </c>
-      <c r="R7" t="s">
-        <v>22</v>
+      <c r="R7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8">
@@ -617,41 +695,41 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" t="b">
-        <v>0</v>
+        <v>49</v>
+      </c>
+      <c r="G8" t="s">
+        <v>34</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
       </c>
       <c r="I8" t="b">
-        <v>1</v>
-      </c>
-      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" t="n">
         <v>62777.0</v>
       </c>
-      <c r="K8" t="n">
-        <v>1.0</v>
-      </c>
       <c r="L8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="M8" t="n">
         <v>21.0</v>
       </c>
-      <c r="M8" t="n">
-        <v>0.0</v>
-      </c>
       <c r="N8" t="n">
         <v>0.0</v>
       </c>
@@ -659,13 +737,16 @@
         <v>0.0</v>
       </c>
       <c r="P8" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q8" t="n">
         <v>1.0</v>
       </c>
-      <c r="R8" t="s">
-        <v>22</v>
+      <c r="R8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="S8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9">
@@ -673,41 +754,41 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" t="b">
-        <v>1</v>
+        <v>52</v>
+      </c>
+      <c r="G9" t="s">
+        <v>46</v>
       </c>
       <c r="H9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" t="n">
         <v>74752.0</v>
       </c>
-      <c r="K9" t="n">
-        <v>1.0</v>
-      </c>
       <c r="L9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="M9" t="n">
         <v>21.0</v>
       </c>
-      <c r="M9" t="n">
-        <v>0.0</v>
-      </c>
       <c r="N9" t="n">
         <v>0.0</v>
       </c>
@@ -715,13 +796,16 @@
         <v>0.0</v>
       </c>
       <c r="P9" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q9" t="n">
         <v>1.0</v>
       </c>
-      <c r="R9" t="s">
-        <v>22</v>
+      <c r="R9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="S9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10">
@@ -729,41 +813,41 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" t="b">
-        <v>0</v>
+        <v>55</v>
+      </c>
+      <c r="G10" t="s">
+        <v>34</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
       </c>
       <c r="I10" t="b">
-        <v>1</v>
-      </c>
-      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="n">
         <v>40138.0</v>
       </c>
-      <c r="K10" t="n">
-        <v>1.0</v>
-      </c>
       <c r="L10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="M10" t="n">
         <v>21.0</v>
       </c>
-      <c r="M10" t="n">
-        <v>0.0</v>
-      </c>
       <c r="N10" t="n">
         <v>0.0</v>
       </c>
@@ -774,10 +858,13 @@
         <v>0.0</v>
       </c>
       <c r="Q10" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="R10" t="s">
-        <v>22</v>
+        <v>0.0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="S10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11">
@@ -785,41 +872,41 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" t="b">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="G11" t="s">
+        <v>46</v>
       </c>
       <c r="H11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" t="n">
         <v>57856.0</v>
       </c>
-      <c r="K11" t="n">
-        <v>1.0</v>
-      </c>
       <c r="L11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="M11" t="n">
         <v>21.0</v>
       </c>
-      <c r="M11" t="n">
-        <v>0.0</v>
-      </c>
       <c r="N11" t="n">
         <v>0.0</v>
       </c>
@@ -830,10 +917,13 @@
         <v>0.0</v>
       </c>
       <c r="Q11" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="R11" t="s">
-        <v>22</v>
+        <v>0.0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="S11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12">
@@ -841,55 +931,58 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" t="b">
-        <v>0</v>
+        <v>62</v>
+      </c>
+      <c r="G12" t="s">
+        <v>34</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
       </c>
       <c r="I12" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" t="n">
         <v>27926.0</v>
       </c>
-      <c r="K12" t="n">
+      <c r="L12" t="n">
         <v>4.0</v>
       </c>
-      <c r="L12" t="n">
+      <c r="M12" t="n">
         <v>224.0</v>
       </c>
-      <c r="M12" t="n">
-        <v>0.0</v>
-      </c>
       <c r="N12" t="n">
         <v>0.0</v>
       </c>
       <c r="O12" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P12" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="Q12" t="n">
         <v>0.0</v>
       </c>
-      <c r="R12" t="s">
-        <v>22</v>
+      <c r="R12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S12" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="13">
@@ -897,41 +990,41 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" t="s">
         <v>46</v>
       </c>
-      <c r="D13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" t="b">
-        <v>1</v>
-      </c>
       <c r="H13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" t="n">
         <v>61440.0</v>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>4.0</v>
       </c>
-      <c r="L13" t="n">
+      <c r="M13" t="n">
         <v>224.0</v>
       </c>
-      <c r="M13" t="n">
-        <v>0.0</v>
-      </c>
       <c r="N13" t="n">
         <v>0.0</v>
       </c>
@@ -944,13 +1037,16 @@
       <c r="Q13" t="n">
         <v>0.0</v>
       </c>
-      <c r="R13" t="s">
-        <v>22</v>
+      <c r="R13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S13" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" sqref="R2:R13" allowBlank="true" errorStyle="stop" showErrorMessage="true">
+    <dataValidation type="list" sqref="S2:S13" allowBlank="true" errorStyle="stop" showErrorMessage="true">
       <formula1>"Auto-Upload,Only-VB-2-Apps,No-Action"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Included logic to auto convert vbscript to app script files
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Infosys\PWC\excel-to-appscript\workspace\eclipse\google\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="summary" r:id="rId3" sheetId="1"/>
+    <sheet name="summary" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
   <si>
     <t>#</t>
   </si>
@@ -210,43 +217,35 @@
   </si>
   <si>
     <t>Thu Jan 19 20:00:06 IST 2017</t>
+  </si>
+  <si>
+    <t>Only-VB-2-Apps</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="C0C0C0"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <bgColor rgb="C0C0C0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="808080"/>
-        <bgColor rgb="C0C0C0"/>
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
   </fills>
@@ -264,21 +263,297 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -336,9 +611,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1.0</v>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
@@ -367,37 +642,37 @@
       <c r="J2" t="b">
         <v>1</v>
       </c>
-      <c r="K2" t="n">
-        <v>899572.0</v>
-      </c>
-      <c r="L2" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="M2" t="n">
-        <v>11937.0</v>
-      </c>
-      <c r="N2" t="n">
-        <v>23.0</v>
-      </c>
-      <c r="O2" t="n">
-        <v>5729.0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="R2" t="n">
-        <v>3.0</v>
+      <c r="K2">
+        <v>899572</v>
+      </c>
+      <c r="L2">
+        <v>14</v>
+      </c>
+      <c r="M2">
+        <v>11937</v>
+      </c>
+      <c r="N2">
+        <v>23</v>
+      </c>
+      <c r="O2">
+        <v>5729</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>3</v>
       </c>
       <c r="S2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2.0</v>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>26</v>
@@ -426,37 +701,37 @@
       <c r="J3" t="b">
         <v>1</v>
       </c>
-      <c r="K3" t="n">
-        <v>505814.0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>19.0</v>
-      </c>
-      <c r="M3" t="n">
-        <v>3323.0</v>
-      </c>
-      <c r="N3" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="O3" t="n">
-        <v>2487.0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0.0</v>
+      <c r="K3">
+        <v>505814</v>
+      </c>
+      <c r="L3">
+        <v>19</v>
+      </c>
+      <c r="M3">
+        <v>3323</v>
+      </c>
+      <c r="N3">
+        <v>11</v>
+      </c>
+      <c r="O3">
+        <v>2487</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
       </c>
       <c r="S3" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3.0</v>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>30</v>
@@ -485,37 +760,37 @@
       <c r="J4" t="b">
         <v>1</v>
       </c>
-      <c r="K4" t="n">
-        <v>16085.0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="M4" t="n">
-        <v>57.0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="R4" t="n">
-        <v>0.0</v>
+      <c r="K4">
+        <v>16085</v>
+      </c>
+      <c r="L4">
+        <v>3</v>
+      </c>
+      <c r="M4">
+        <v>57</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
       </c>
       <c r="S4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4.0</v>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>35</v>
@@ -544,37 +819,37 @@
       <c r="J5" t="b">
         <v>1</v>
       </c>
-      <c r="K5" t="n">
-        <v>12236.0</v>
-      </c>
-      <c r="L5" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="M5" t="n">
-        <v>38.0</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0.0</v>
+      <c r="K5">
+        <v>12236</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>38</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
       </c>
       <c r="S5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5.0</v>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>39</v>
@@ -603,37 +878,37 @@
       <c r="J6" t="b">
         <v>1</v>
       </c>
-      <c r="K6" t="n">
-        <v>18789.0</v>
-      </c>
-      <c r="L6" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="M6" t="n">
-        <v>43.0</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="R6" t="n">
-        <v>0.0</v>
+      <c r="K6">
+        <v>18789</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>43</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
       </c>
       <c r="S6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6.0</v>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>43</v>
@@ -662,37 +937,37 @@
       <c r="J7" t="b">
         <v>1</v>
       </c>
-      <c r="K7" t="n">
-        <v>39936.0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="M7" t="n">
-        <v>43.0</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="R7" t="n">
-        <v>0.0</v>
+      <c r="K7">
+        <v>39936</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <v>43</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
       </c>
       <c r="S7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7.0</v>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>47</v>
@@ -721,37 +996,37 @@
       <c r="J8" t="b">
         <v>1</v>
       </c>
-      <c r="K8" t="n">
-        <v>62777.0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="M8" t="n">
-        <v>21.0</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="R8" t="n">
-        <v>1.0</v>
+      <c r="K8">
+        <v>62777</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>21</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
       </c>
       <c r="S8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8.0</v>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>50</v>
@@ -780,37 +1055,37 @@
       <c r="J9" t="b">
         <v>1</v>
       </c>
-      <c r="K9" t="n">
-        <v>74752.0</v>
-      </c>
-      <c r="L9" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="M9" t="n">
-        <v>21.0</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P9" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="R9" t="n">
-        <v>1.0</v>
+      <c r="K9">
+        <v>74752</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>21</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
       </c>
       <c r="S9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9.0</v>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>53</v>
@@ -839,37 +1114,37 @@
       <c r="J10" t="b">
         <v>1</v>
       </c>
-      <c r="K10" t="n">
-        <v>40138.0</v>
-      </c>
-      <c r="L10" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="M10" t="n">
-        <v>21.0</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O10" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P10" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="R10" t="n">
-        <v>1.0</v>
+      <c r="K10">
+        <v>40138</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>21</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
       </c>
       <c r="S10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10.0</v>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>56</v>
@@ -898,37 +1173,37 @@
       <c r="J11" t="b">
         <v>1</v>
       </c>
-      <c r="K11" t="n">
-        <v>57856.0</v>
-      </c>
-      <c r="L11" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="M11" t="n">
-        <v>21.0</v>
-      </c>
-      <c r="N11" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O11" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="R11" t="n">
-        <v>1.0</v>
+      <c r="K11">
+        <v>57856</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>21</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
       </c>
       <c r="S11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11.0</v>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>59</v>
@@ -957,37 +1232,37 @@
       <c r="J12" t="b">
         <v>1</v>
       </c>
-      <c r="K12" t="n">
-        <v>27926.0</v>
-      </c>
-      <c r="L12" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="M12" t="n">
-        <v>224.0</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P12" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="R12" t="n">
-        <v>0.0</v>
+      <c r="K12">
+        <v>27926</v>
+      </c>
+      <c r="L12">
+        <v>4</v>
+      </c>
+      <c r="M12">
+        <v>224</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
       </c>
       <c r="S12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12.0</v>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>63</v>
@@ -1016,29 +1291,29 @@
       <c r="J13" t="b">
         <v>1</v>
       </c>
-      <c r="K13" t="n">
-        <v>61440.0</v>
-      </c>
-      <c r="L13" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="M13" t="n">
-        <v>224.0</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="R13" t="n">
-        <v>0.0</v>
+      <c r="K13">
+        <v>61440</v>
+      </c>
+      <c r="L13">
+        <v>4</v>
+      </c>
+      <c r="M13">
+        <v>224</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
       </c>
       <c r="S13" t="s">
         <v>25</v>
@@ -1046,10 +1321,10 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" sqref="S2:S13" allowBlank="true" errorStyle="stop" showErrorMessage="true">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="S2:S13">
       <formula1>"Auto-Upload,Only-VB-2-Apps,No-Action"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>